<commit_message>
Deploying to gh-pages from  @ 51cdd5e54f2d76c84826e4c33ed210c68f00e6b1 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_5-3-1.xlsx
+++ b/assets/excel/2021_5-3-1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring_2021\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2C2A54-5A65-43EF-AAD4-7E6D3BF59400}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF989A9F-A4FF-49EE-A66F-1FD6A48FB8E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{33FB2155-6077-45A0-8E99-4914181CDB70}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="29">
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
   </si>
@@ -124,13 +124,17 @@
   <si>
     <t>https://www.destatis.de/DE/Themen/Gesellschaft-Umwelt/Bevoelkerung/Haushalte-Familien/Methoden/mikrozensus-2020.html</t>
   </si>
+  <si>
+    <t>/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="\(0.0\)"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -182,12 +186,18 @@
       <name val="NDSFrutiger 55 Roman"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -251,10 +261,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -277,17 +287,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -310,41 +311,77 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Link 2" xfId="2" xr:uid="{D2133F87-399F-410A-B3BD-7D7FAC665F4E}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard_Tabelle_A_6_HT" xfId="2" xr:uid="{124C7E12-BB24-403E-BF77-B06B84633AE0}"/>
+    <cellStyle name="Standard_Tabelle_A_6_HT" xfId="1" xr:uid="{124C7E12-BB24-403E-BF77-B06B84633AE0}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -660,13 +697,13 @@
   <dimension ref="A1:AD42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="14" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="14"/>
+    <col min="1" max="1" width="5.7109375" style="11" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -796,288 +833,288 @@
       <c r="AD5" s="7"/>
     </row>
     <row r="6" spans="1:30" s="9" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="27"/>
-      <c r="V6" s="27"/>
-      <c r="W6" s="27"/>
-      <c r="X6" s="27"/>
-      <c r="Y6" s="27"/>
-      <c r="Z6" s="27"/>
-      <c r="AA6" s="27"/>
-      <c r="AB6" s="27"/>
-      <c r="AC6" s="27"/>
-      <c r="AD6" s="28"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
+      <c r="W6" s="20"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="20"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="20"/>
+      <c r="AD6" s="21"/>
     </row>
     <row r="7" spans="1:30" s="9" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-      <c r="C7" s="29" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="20">
         <v>2019</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27">
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20">
         <v>2018</v>
       </c>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27">
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20">
         <v>2017</v>
       </c>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27">
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20">
         <v>2016</v>
       </c>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27">
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20">
         <v>2015</v>
       </c>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27">
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20">
         <v>2014</v>
       </c>
-      <c r="T7" s="27"/>
-      <c r="U7" s="27"/>
-      <c r="V7" s="27">
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20">
         <v>2013</v>
       </c>
-      <c r="W7" s="27"/>
-      <c r="X7" s="27"/>
-      <c r="Y7" s="27">
+      <c r="W7" s="20"/>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="20">
         <v>2012</v>
       </c>
-      <c r="Z7" s="27"/>
-      <c r="AA7" s="27"/>
-      <c r="AB7" s="27">
+      <c r="Z7" s="20"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20">
         <v>2011</v>
       </c>
-      <c r="AC7" s="27"/>
-      <c r="AD7" s="28"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="21"/>
     </row>
     <row r="8" spans="1:30" s="9" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="27" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="27" t="s">
+      <c r="J8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="K8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="27" t="s">
+      <c r="L8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="M8" s="27" t="s">
+      <c r="M8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="N8" s="27" t="s">
+      <c r="N8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="O8" s="27" t="s">
+      <c r="O8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="27" t="s">
+      <c r="P8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="Q8" s="27" t="s">
+      <c r="Q8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="R8" s="27" t="s">
+      <c r="R8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="S8" s="27" t="s">
+      <c r="S8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="T8" s="27" t="s">
+      <c r="T8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="U8" s="27" t="s">
+      <c r="U8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="V8" s="27" t="s">
+      <c r="V8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="W8" s="27" t="s">
+      <c r="W8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="X8" s="27" t="s">
+      <c r="X8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="Y8" s="27" t="s">
+      <c r="Y8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="Z8" s="27" t="s">
+      <c r="Z8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="AA8" s="27" t="s">
+      <c r="AA8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="AB8" s="27" t="s">
+      <c r="AB8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="AC8" s="27" t="s">
+      <c r="AC8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="AD8" s="28" t="s">
+      <c r="AD8" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:30" s="9" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="26"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="27"/>
-      <c r="V9" s="27"/>
-      <c r="W9" s="27"/>
-      <c r="X9" s="27"/>
-      <c r="Y9" s="27"/>
-      <c r="Z9" s="27"/>
-      <c r="AA9" s="27"/>
-      <c r="AB9" s="27"/>
-      <c r="AC9" s="27"/>
-      <c r="AD9" s="28"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="21"/>
     </row>
     <row r="10" spans="1:30" s="9" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27" t="s">
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27" t="s">
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27" t="s">
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27" t="s">
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27" t="s">
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="R10" s="27"/>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27" t="s">
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="U10" s="27"/>
-      <c r="V10" s="27"/>
-      <c r="W10" s="27" t="s">
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="X10" s="27"/>
-      <c r="Y10" s="27"/>
-      <c r="Z10" s="27" t="s">
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20"/>
+      <c r="Z10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="AA10" s="27"/>
-      <c r="AB10" s="27"/>
-      <c r="AC10" s="27" t="s">
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="AD10" s="28"/>
+      <c r="AD10" s="21"/>
     </row>
     <row r="11" spans="1:30" s="9" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="27" t="s">
+      <c r="B11" s="24"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
-      <c r="U11" s="27"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="27"/>
-      <c r="X11" s="27"/>
-      <c r="Y11" s="27"/>
-      <c r="Z11" s="27"/>
-      <c r="AA11" s="27"/>
-      <c r="AB11" s="27"/>
-      <c r="AC11" s="27"/>
-      <c r="AD11" s="28"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="20"/>
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="20"/>
+      <c r="AC11" s="20"/>
+      <c r="AD11" s="21"/>
     </row>
     <row r="12" spans="1:30" s="9" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
@@ -1170,1776 +1207,1813 @@
     </row>
     <row r="13" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="28">
         <v>3.21</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="28">
         <v>2.6</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="28">
         <v>4.78</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="28">
         <v>3.15</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="28">
         <v>2.82</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="28">
         <v>4.03</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="28">
         <v>3.15</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13" s="28">
         <v>2.4900000000000002</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="28">
         <v>4.84</v>
       </c>
-      <c r="M13" s="13">
+      <c r="M13" s="28">
         <v>3.36</v>
       </c>
-      <c r="N13" s="13">
+      <c r="N13" s="28">
         <v>3.01</v>
       </c>
-      <c r="O13" s="13">
+      <c r="O13" s="28">
         <v>4.45</v>
       </c>
-      <c r="P13" s="13">
+      <c r="P13" s="29">
         <v>3.03</v>
       </c>
-      <c r="Q13" s="13">
+      <c r="Q13" s="29">
         <v>2.88</v>
       </c>
-      <c r="R13" s="13">
+      <c r="R13" s="29">
         <v>3.56</v>
       </c>
-      <c r="S13" s="13">
+      <c r="S13" s="30">
         <v>3.36</v>
       </c>
-      <c r="T13" s="13">
+      <c r="T13" s="30">
         <v>3.14</v>
       </c>
-      <c r="U13" s="13">
+      <c r="U13" s="31">
         <v>4.1900000000000004</v>
       </c>
-      <c r="V13" s="13">
+      <c r="V13" s="30">
         <v>3.92</v>
       </c>
-      <c r="W13" s="13">
+      <c r="W13" s="30">
         <v>3.84</v>
       </c>
-      <c r="X13" s="13">
+      <c r="X13" s="31">
         <v>4.17</v>
       </c>
-      <c r="Y13" s="13">
+      <c r="Y13" s="30">
         <v>3.79</v>
       </c>
-      <c r="Z13" s="13">
+      <c r="Z13" s="30">
         <v>3.49</v>
       </c>
-      <c r="AA13" s="13">
+      <c r="AA13" s="32">
         <v>4.8899999999999997</v>
       </c>
-      <c r="AB13" s="13">
+      <c r="AB13" s="30">
         <v>4.76</v>
       </c>
-      <c r="AC13" s="13">
+      <c r="AC13" s="30">
         <v>4.75</v>
       </c>
-      <c r="AD13" s="13">
+      <c r="AD13" s="30">
         <v>4.78</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="28">
         <v>3.59</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="28">
         <v>2.9</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="28">
         <v>5.24</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="28">
         <v>3.68</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="28">
         <v>3.02</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="28">
         <v>5.24</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="28">
         <v>4.03</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K14" s="28">
         <v>3.22</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="28">
         <v>5.87</v>
       </c>
-      <c r="M14" s="13">
+      <c r="M14" s="28">
         <v>4.5199999999999996</v>
       </c>
-      <c r="N14" s="13">
+      <c r="N14" s="28">
         <v>4</v>
       </c>
-      <c r="O14" s="13">
+      <c r="O14" s="28">
         <v>5.94</v>
       </c>
-      <c r="P14" s="13">
+      <c r="P14" s="29">
         <v>4.33</v>
       </c>
-      <c r="Q14" s="13">
+      <c r="Q14" s="29">
         <v>3.79</v>
       </c>
-      <c r="R14" s="13">
+      <c r="R14" s="29">
         <v>6.16</v>
       </c>
-      <c r="S14" s="13">
+      <c r="S14" s="30">
         <v>4.8600000000000003</v>
       </c>
-      <c r="T14" s="13">
+      <c r="T14" s="30">
         <v>4.53</v>
       </c>
-      <c r="U14" s="13">
+      <c r="U14" s="30">
         <v>5.97</v>
       </c>
-      <c r="V14" s="13">
+      <c r="V14" s="30">
         <v>4.95</v>
       </c>
-      <c r="W14" s="13">
+      <c r="W14" s="30">
         <v>4.63</v>
       </c>
-      <c r="X14" s="13">
+      <c r="X14" s="31">
         <v>5.89</v>
       </c>
-      <c r="Y14" s="13">
+      <c r="Y14" s="30">
         <v>4.62</v>
       </c>
-      <c r="Z14" s="13">
+      <c r="Z14" s="30">
         <v>4.07</v>
       </c>
-      <c r="AA14" s="13">
+      <c r="AA14" s="30">
         <v>6.49</v>
       </c>
-      <c r="AB14" s="13">
+      <c r="AB14" s="30">
         <v>5.0999999999999996</v>
       </c>
-      <c r="AC14" s="13">
+      <c r="AC14" s="30">
         <v>4.5999999999999996</v>
       </c>
-      <c r="AD14" s="13">
+      <c r="AD14" s="30">
         <v>6.84</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="28">
         <v>2.44</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="28">
         <v>1.78</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="28">
         <v>3.98</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="28">
         <v>2.5499999999999998</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="28">
         <v>1.7</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="28">
         <v>4.4800000000000004</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="28">
         <v>2.92</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K15" s="28">
         <v>2.16</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15" s="28">
         <v>4.75</v>
       </c>
-      <c r="M15" s="13">
+      <c r="M15" s="28">
         <v>3.32</v>
       </c>
-      <c r="N15" s="13">
+      <c r="N15" s="28">
         <v>2.44</v>
       </c>
-      <c r="O15" s="13">
+      <c r="O15" s="28">
         <v>6</v>
       </c>
-      <c r="P15" s="13">
+      <c r="P15" s="29">
         <v>3.52</v>
       </c>
-      <c r="Q15" s="13">
+      <c r="Q15" s="29">
         <v>3.06</v>
       </c>
-      <c r="R15" s="13">
+      <c r="R15" s="29">
         <v>5.1100000000000003</v>
       </c>
-      <c r="S15" s="13">
+      <c r="S15" s="30">
         <v>3.68</v>
       </c>
-      <c r="T15" s="13">
+      <c r="T15" s="30">
         <v>3.23</v>
       </c>
-      <c r="U15" s="13">
+      <c r="U15" s="30">
         <v>5.41</v>
       </c>
-      <c r="V15" s="13">
+      <c r="V15" s="30">
         <v>3.94</v>
       </c>
-      <c r="W15" s="13">
+      <c r="W15" s="30">
         <v>3.48</v>
       </c>
-      <c r="X15" s="13">
+      <c r="X15" s="31">
         <v>5.71</v>
       </c>
-      <c r="Y15" s="13">
+      <c r="Y15" s="30">
         <v>3.69</v>
       </c>
-      <c r="Z15" s="13">
+      <c r="Z15" s="30">
         <v>3.2</v>
       </c>
-      <c r="AA15" s="13">
+      <c r="AA15" s="30">
         <v>6.02</v>
       </c>
-      <c r="AB15" s="13">
+      <c r="AB15" s="30">
         <v>3.78</v>
       </c>
-      <c r="AC15" s="13">
+      <c r="AC15" s="30">
         <v>3.25</v>
       </c>
-      <c r="AD15" s="13">
+      <c r="AD15" s="30">
         <v>6.33</v>
       </c>
     </row>
     <row r="16" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="28">
         <v>1.84</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="28">
         <v>1.5</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="33">
         <v>3.32</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="28">
         <v>2.08</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="28">
         <v>1.8</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="33">
         <v>3.36</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="28">
         <v>2.59</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K16" s="28">
         <v>2.13</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="28">
         <v>4.82</v>
       </c>
-      <c r="M16" s="13">
+      <c r="M16" s="28">
         <v>2.46</v>
       </c>
-      <c r="N16" s="13">
+      <c r="N16" s="28">
         <v>2.16</v>
       </c>
-      <c r="O16" s="13">
+      <c r="O16" s="33">
         <v>4.13</v>
       </c>
-      <c r="P16" s="13">
+      <c r="P16" s="29">
         <v>3.27</v>
       </c>
-      <c r="Q16" s="13">
+      <c r="Q16" s="29">
         <v>2.91</v>
       </c>
-      <c r="R16" s="13">
+      <c r="R16" s="29">
         <v>5.45</v>
       </c>
-      <c r="S16" s="13">
+      <c r="S16" s="30">
         <v>3.39</v>
       </c>
-      <c r="T16" s="13">
+      <c r="T16" s="30">
         <v>3</v>
       </c>
-      <c r="U16" s="13">
+      <c r="U16" s="30">
         <v>5.71</v>
       </c>
-      <c r="V16" s="13">
+      <c r="V16" s="30">
         <v>3.36</v>
       </c>
-      <c r="W16" s="13">
+      <c r="W16" s="30">
         <v>2.99</v>
       </c>
-      <c r="X16" s="13">
+      <c r="X16" s="31">
         <v>5.5</v>
       </c>
-      <c r="Y16" s="13">
+      <c r="Y16" s="30">
         <v>3.64</v>
       </c>
-      <c r="Z16" s="13">
+      <c r="Z16" s="30">
         <v>3.13</v>
       </c>
-      <c r="AA16" s="13">
+      <c r="AA16" s="30">
         <v>6.82</v>
       </c>
-      <c r="AB16" s="13">
+      <c r="AB16" s="30">
         <v>4.2</v>
       </c>
-      <c r="AC16" s="13">
+      <c r="AC16" s="30">
         <v>3.69</v>
       </c>
-      <c r="AD16" s="13">
+      <c r="AD16" s="30">
         <v>7.42</v>
       </c>
     </row>
     <row r="17" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="28">
         <v>1.75</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="28">
         <v>1.53</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="33">
         <v>2.96</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="28">
         <v>1.97</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="28">
         <v>1.86</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="28">
         <v>2.6</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="28">
         <v>2.37</v>
       </c>
-      <c r="K17" s="13">
+      <c r="K17" s="28">
         <v>2.09</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="33">
         <v>3.92</v>
       </c>
-      <c r="M17" s="13">
+      <c r="M17" s="28">
         <v>2.46</v>
       </c>
-      <c r="N17" s="13">
+      <c r="N17" s="28">
         <v>2.15</v>
       </c>
-      <c r="O17" s="13">
+      <c r="O17" s="33">
         <v>4.3099999999999996</v>
       </c>
-      <c r="P17" s="13">
+      <c r="P17" s="29">
         <v>2.61</v>
       </c>
-      <c r="Q17" s="13">
+      <c r="Q17" s="29">
         <v>2.2400000000000002</v>
       </c>
-      <c r="R17" s="13">
+      <c r="R17" s="34">
         <v>4.88</v>
       </c>
-      <c r="S17" s="13">
+      <c r="S17" s="30">
         <v>3.07</v>
       </c>
-      <c r="T17" s="13">
+      <c r="T17" s="30">
         <v>2.72</v>
       </c>
-      <c r="U17" s="13">
+      <c r="U17" s="35">
         <v>5.32</v>
       </c>
-      <c r="V17" s="13">
+      <c r="V17" s="30">
         <v>3.19</v>
       </c>
-      <c r="W17" s="13">
+      <c r="W17" s="30">
         <v>2.79</v>
       </c>
-      <c r="X17" s="13">
+      <c r="X17" s="35">
         <v>5.66</v>
       </c>
-      <c r="Y17" s="13">
+      <c r="Y17" s="30">
         <v>3.22</v>
       </c>
-      <c r="Z17" s="13">
+      <c r="Z17" s="30">
         <v>2.72</v>
       </c>
-      <c r="AA17" s="13">
+      <c r="AA17" s="32">
         <v>6.36</v>
       </c>
-      <c r="AB17" s="13">
+      <c r="AB17" s="30">
         <v>3.56</v>
       </c>
-      <c r="AC17" s="13">
+      <c r="AC17" s="30">
         <v>2.92</v>
       </c>
-      <c r="AD17" s="13">
+      <c r="AD17" s="30">
         <v>7.84</v>
       </c>
     </row>
     <row r="18" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="28">
         <v>2.48</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="28">
         <v>1.96</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="28">
         <v>4.16</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="28">
         <v>2.62</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="28">
         <v>2.17</v>
       </c>
-      <c r="I18" s="13">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="J18" s="13">
+      <c r="I18" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="28">
         <v>2.96</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K18" s="28">
         <v>2.36</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L18" s="28">
         <v>4.93</v>
       </c>
-      <c r="M18" s="13">
+      <c r="M18" s="28">
         <v>3.15</v>
       </c>
-      <c r="N18" s="13">
+      <c r="N18" s="28">
         <v>2.65</v>
       </c>
-      <c r="O18" s="13">
+      <c r="O18" s="28">
         <v>5.07</v>
       </c>
-      <c r="P18" s="13">
+      <c r="P18" s="29">
         <v>3.33</v>
       </c>
-      <c r="Q18" s="13">
+      <c r="Q18" s="29">
         <v>2.93</v>
       </c>
-      <c r="R18" s="13">
+      <c r="R18" s="29">
         <v>5.07</v>
       </c>
-      <c r="S18" s="13">
+      <c r="S18" s="30">
         <v>3.64</v>
       </c>
-      <c r="T18" s="13">
+      <c r="T18" s="30">
         <v>3.26</v>
       </c>
-      <c r="U18" s="13">
+      <c r="U18" s="30">
         <v>5.34</v>
       </c>
-      <c r="V18" s="13">
+      <c r="V18" s="30">
         <v>3.81</v>
       </c>
-      <c r="W18" s="13">
+      <c r="W18" s="30">
         <v>3.44</v>
       </c>
-      <c r="X18" s="13">
+      <c r="X18" s="30">
         <v>5.38</v>
       </c>
-      <c r="Y18" s="13">
+      <c r="Y18" s="30">
         <v>3.76</v>
       </c>
-      <c r="Z18" s="13">
+      <c r="Z18" s="30">
         <v>3.27</v>
       </c>
-      <c r="AA18" s="13">
+      <c r="AA18" s="30">
         <v>6.11</v>
       </c>
-      <c r="AB18" s="13">
+      <c r="AB18" s="30">
         <v>4.2300000000000004</v>
       </c>
-      <c r="AC18" s="13">
+      <c r="AC18" s="30">
         <v>3.76</v>
       </c>
-      <c r="AD18" s="13">
+      <c r="AD18" s="30">
         <v>6.55</v>
       </c>
     </row>
     <row r="19" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="28">
         <v>3.55</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="33">
         <v>2.86</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="33">
         <v>5.24</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="28">
         <v>3.48</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="33">
         <v>2.84</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="33">
         <v>5.09</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="28">
         <v>3.69</v>
       </c>
-      <c r="K19" s="13">
+      <c r="K19" s="33">
         <v>2.94</v>
       </c>
-      <c r="L19" s="13">
+      <c r="L19" s="33">
         <v>5.46</v>
       </c>
-      <c r="M19" s="13">
+      <c r="M19" s="28">
         <v>4.1100000000000003</v>
       </c>
-      <c r="N19" s="13">
+      <c r="N19" s="28">
         <v>3.58</v>
       </c>
-      <c r="O19" s="13">
+      <c r="O19" s="33">
         <v>5.61</v>
       </c>
-      <c r="P19" s="13">
+      <c r="P19" s="29">
         <v>3.38</v>
       </c>
-      <c r="Q19" s="13">
+      <c r="Q19" s="29">
         <v>3.27</v>
       </c>
-      <c r="R19" s="13">
-        <v>3.72</v>
-      </c>
-      <c r="S19" s="13">
+      <c r="R19" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="S19" s="30">
         <v>3.98</v>
       </c>
-      <c r="T19" s="13">
+      <c r="T19" s="30">
         <v>3.97</v>
       </c>
-      <c r="U19" s="13">
-        <v>4.04</v>
-      </c>
-      <c r="V19" s="13">
+      <c r="U19" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="V19" s="30">
         <v>4.29</v>
       </c>
-      <c r="W19" s="13">
+      <c r="W19" s="30">
         <v>4.0999999999999996</v>
       </c>
-      <c r="X19" s="13">
+      <c r="X19" s="35">
         <v>4.92</v>
       </c>
-      <c r="Y19" s="13">
+      <c r="Y19" s="30">
         <v>4.03</v>
       </c>
-      <c r="Z19" s="13">
+      <c r="Z19" s="30">
         <v>3.75</v>
       </c>
-      <c r="AA19" s="13">
-        <v>5.04</v>
-      </c>
-      <c r="AB19" s="13">
+      <c r="AA19" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB19" s="30">
         <v>5.25</v>
       </c>
-      <c r="AC19" s="13">
+      <c r="AC19" s="30">
         <v>5.08</v>
       </c>
-      <c r="AD19" s="13">
+      <c r="AD19" s="30">
         <v>5.85</v>
       </c>
     </row>
     <row r="20" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="28">
         <v>4.6399999999999997</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="28">
         <v>3.6</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="28">
         <v>6.96</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="28">
         <v>4.32</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="28">
         <v>3.49</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="33">
         <v>6.22</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="28">
         <v>4.8899999999999997</v>
       </c>
-      <c r="K20" s="13">
+      <c r="K20" s="28">
         <v>3.64</v>
       </c>
-      <c r="L20" s="13">
+      <c r="L20" s="28">
         <v>7.53</v>
       </c>
-      <c r="M20" s="13">
+      <c r="M20" s="28">
         <v>5.37</v>
       </c>
-      <c r="N20" s="13">
+      <c r="N20" s="28">
         <v>4.5199999999999996</v>
       </c>
-      <c r="O20" s="13">
+      <c r="O20" s="28">
         <v>7.57</v>
       </c>
-      <c r="P20" s="13">
+      <c r="P20" s="29">
         <v>5.26</v>
       </c>
-      <c r="Q20" s="13">
+      <c r="Q20" s="29">
         <v>4.91</v>
       </c>
-      <c r="R20" s="13">
+      <c r="R20" s="34">
         <v>6.44</v>
       </c>
-      <c r="S20" s="13">
+      <c r="S20" s="30">
         <v>5.71</v>
       </c>
-      <c r="T20" s="13">
+      <c r="T20" s="30">
         <v>5.38</v>
       </c>
-      <c r="U20" s="13">
+      <c r="U20" s="35">
         <v>6.78</v>
       </c>
-      <c r="V20" s="13">
+      <c r="V20" s="30">
         <v>6.14</v>
       </c>
-      <c r="W20" s="13">
+      <c r="W20" s="30">
         <v>5.68</v>
       </c>
-      <c r="X20" s="13">
+      <c r="X20" s="35">
         <v>7.53</v>
       </c>
-      <c r="Y20" s="13">
+      <c r="Y20" s="30">
         <v>5.43</v>
       </c>
-      <c r="Z20" s="13">
+      <c r="Z20" s="30">
         <v>4.71</v>
       </c>
-      <c r="AA20" s="13">
+      <c r="AA20" s="32">
         <v>7.91</v>
       </c>
-      <c r="AB20" s="13">
+      <c r="AB20" s="30">
         <v>5.37</v>
       </c>
-      <c r="AC20" s="13">
+      <c r="AC20" s="30">
         <v>4.45</v>
       </c>
-      <c r="AD20" s="13">
+      <c r="AD20" s="30">
         <v>8.4700000000000006</v>
       </c>
     </row>
     <row r="21" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="28">
         <v>2.85</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="33">
         <v>2.04</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="33">
         <v>4.63</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="28">
         <v>3.19</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="33">
         <v>2.1</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="33">
         <v>5.47</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J21" s="28">
         <v>3.07</v>
       </c>
-      <c r="K21" s="13">
+      <c r="K21" s="33">
         <v>2.21</v>
       </c>
-      <c r="L21" s="13">
+      <c r="L21" s="33">
         <v>5.09</v>
       </c>
-      <c r="M21" s="13">
+      <c r="M21" s="28">
         <v>4.12</v>
       </c>
-      <c r="N21" s="13">
+      <c r="N21" s="28">
         <v>2.88</v>
       </c>
-      <c r="O21" s="13">
+      <c r="O21" s="33">
         <v>7.82</v>
       </c>
-      <c r="P21" s="13">
+      <c r="P21" s="29">
         <v>3.9</v>
       </c>
-      <c r="Q21" s="13">
+      <c r="Q21" s="29">
         <v>3.41</v>
       </c>
-      <c r="R21" s="13">
+      <c r="R21" s="34">
         <v>5.56</v>
       </c>
-      <c r="S21" s="13">
+      <c r="S21" s="30">
         <v>4.25</v>
       </c>
-      <c r="T21" s="13">
+      <c r="T21" s="30">
         <v>3.69</v>
       </c>
-      <c r="U21" s="13">
+      <c r="U21" s="35">
         <v>6.5</v>
       </c>
-      <c r="V21" s="13">
+      <c r="V21" s="30">
         <v>4.5199999999999996</v>
       </c>
-      <c r="W21" s="13">
+      <c r="W21" s="30">
         <v>3.87</v>
       </c>
-      <c r="X21" s="13">
+      <c r="X21" s="35">
         <v>6.97</v>
       </c>
-      <c r="Y21" s="13">
+      <c r="Y21" s="30">
         <v>4.25</v>
       </c>
-      <c r="Z21" s="13">
+      <c r="Z21" s="30">
         <v>3.41</v>
       </c>
-      <c r="AA21" s="13">
+      <c r="AA21" s="32">
         <v>8.32</v>
       </c>
-      <c r="AB21" s="13">
+      <c r="AB21" s="30">
         <v>3.81</v>
       </c>
-      <c r="AC21" s="13">
+      <c r="AC21" s="30">
         <v>3.23</v>
       </c>
-      <c r="AD21" s="13">
+      <c r="AD21" s="30">
         <v>6.8</v>
       </c>
     </row>
     <row r="22" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="28">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="33">
         <v>1.97</v>
       </c>
-      <c r="F22" s="13">
-        <v>3.78</v>
-      </c>
-      <c r="G22" s="13">
+      <c r="F22" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="28">
         <v>2.31</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="28">
         <v>2.08</v>
       </c>
-      <c r="I22" s="13">
-        <v>3.39</v>
-      </c>
-      <c r="J22" s="13">
+      <c r="I22" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J22" s="28">
         <v>3.09</v>
       </c>
-      <c r="K22" s="13">
+      <c r="K22" s="28">
         <v>2.5499999999999998</v>
       </c>
-      <c r="L22" s="13">
+      <c r="L22" s="33">
         <v>5.56</v>
       </c>
-      <c r="M22" s="13">
+      <c r="M22" s="28">
         <v>2.89</v>
       </c>
-      <c r="N22" s="13">
+      <c r="N22" s="28">
         <v>2.42</v>
       </c>
-      <c r="O22" s="13">
+      <c r="O22" s="33">
         <v>5.49</v>
       </c>
-      <c r="P22" s="13">
+      <c r="P22" s="29">
         <v>3.51</v>
       </c>
-      <c r="Q22" s="13">
+      <c r="Q22" s="29">
         <v>3.03</v>
       </c>
-      <c r="R22" s="13">
+      <c r="R22" s="34">
         <v>6.3</v>
       </c>
-      <c r="S22" s="13">
+      <c r="S22" s="30">
         <v>3.77</v>
       </c>
-      <c r="T22" s="13">
+      <c r="T22" s="30">
         <v>3.26</v>
       </c>
-      <c r="U22" s="13">
+      <c r="U22" s="35">
         <v>6.71</v>
       </c>
-      <c r="V22" s="13">
+      <c r="V22" s="30">
         <v>3.54</v>
       </c>
-      <c r="W22" s="13">
+      <c r="W22" s="30">
         <v>3.04</v>
       </c>
-      <c r="X22" s="13">
+      <c r="X22" s="35">
         <v>6.47</v>
       </c>
-      <c r="Y22" s="13">
+      <c r="Y22" s="30">
         <v>3.91</v>
       </c>
-      <c r="Z22" s="13">
+      <c r="Z22" s="30">
         <v>3.22</v>
       </c>
-      <c r="AA22" s="13">
+      <c r="AA22" s="32">
         <v>8.19</v>
       </c>
-      <c r="AB22" s="13">
+      <c r="AB22" s="30">
         <v>4.4800000000000004</v>
       </c>
-      <c r="AC22" s="13">
+      <c r="AC22" s="30">
         <v>3.73</v>
       </c>
-      <c r="AD22" s="13">
+      <c r="AD22" s="30">
         <v>9.35</v>
       </c>
     </row>
     <row r="23" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="28">
         <v>2.16</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="33">
         <v>1.81</v>
       </c>
-      <c r="F23" s="13">
-        <v>4.03</v>
-      </c>
-      <c r="G23" s="13">
+      <c r="F23" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="28">
         <v>2.37</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="28">
         <v>2.1800000000000002</v>
       </c>
-      <c r="I23" s="13">
-        <v>3.42</v>
-      </c>
-      <c r="J23" s="13">
+      <c r="I23" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="28">
         <v>2.81</v>
       </c>
-      <c r="K23" s="13">
+      <c r="K23" s="28">
         <v>2.4300000000000002</v>
       </c>
-      <c r="L23" s="13">
-        <v>4.93</v>
-      </c>
-      <c r="M23" s="13">
+      <c r="L23" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="M23" s="28">
         <v>2.98</v>
       </c>
-      <c r="N23" s="13">
+      <c r="N23" s="28">
         <v>2.63</v>
       </c>
-      <c r="O23" s="13">
-        <v>5.09</v>
-      </c>
-      <c r="P23" s="13">
+      <c r="O23" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="P23" s="29">
         <v>3.16</v>
       </c>
-      <c r="Q23" s="13">
+      <c r="Q23" s="29">
         <v>2.5499999999999998</v>
       </c>
-      <c r="R23" s="13">
-        <v>7.1</v>
-      </c>
-      <c r="S23" s="13">
+      <c r="R23" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="S23" s="30">
         <v>3.84</v>
       </c>
-      <c r="T23" s="13">
+      <c r="T23" s="30">
         <v>3.31</v>
       </c>
-      <c r="U23" s="13">
-        <v>7.33</v>
-      </c>
-      <c r="V23" s="13">
+      <c r="U23" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="V23" s="30">
         <v>3.8</v>
       </c>
-      <c r="W23" s="13">
+      <c r="W23" s="30">
         <v>3.03</v>
       </c>
-      <c r="X23" s="13">
+      <c r="X23" s="35">
         <v>8.39</v>
       </c>
-      <c r="Y23" s="13">
+      <c r="Y23" s="30">
         <v>3.92</v>
       </c>
-      <c r="Z23" s="13">
+      <c r="Z23" s="30">
         <v>3.28</v>
       </c>
-      <c r="AA23" s="13">
+      <c r="AA23" s="32">
         <v>8.0299999999999994</v>
       </c>
-      <c r="AB23" s="13">
+      <c r="AB23" s="30">
         <v>4.01</v>
       </c>
-      <c r="AC23" s="13">
+      <c r="AC23" s="30">
         <v>3.27</v>
       </c>
-      <c r="AD23" s="13">
+      <c r="AD23" s="30">
         <v>9.18</v>
       </c>
     </row>
     <row r="24" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="28">
         <v>3.03</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="28">
         <v>2.37</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="28">
         <v>5.09</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="28">
         <v>3.06</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="28">
         <v>2.48</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="28">
         <v>4.92</v>
       </c>
-      <c r="J24" s="13">
+      <c r="J24" s="28">
         <v>3.48</v>
       </c>
-      <c r="K24" s="13">
+      <c r="K24" s="28">
         <v>2.72</v>
       </c>
-      <c r="L24" s="13">
+      <c r="L24" s="28">
         <v>5.85</v>
       </c>
-      <c r="M24" s="13">
+      <c r="M24" s="28">
         <v>3.81</v>
       </c>
-      <c r="N24" s="13">
+      <c r="N24" s="28">
         <v>3.1</v>
       </c>
-      <c r="O24" s="13">
+      <c r="O24" s="28">
         <v>6.47</v>
       </c>
-      <c r="P24" s="13">
+      <c r="P24" s="29">
         <v>3.8</v>
       </c>
-      <c r="Q24" s="13">
+      <c r="Q24" s="29">
         <v>3.36</v>
       </c>
-      <c r="R24" s="13">
+      <c r="R24" s="36">
         <v>5.75</v>
       </c>
-      <c r="S24" s="13">
+      <c r="S24" s="30">
         <v>4.26</v>
       </c>
-      <c r="T24" s="13">
+      <c r="T24" s="30">
         <v>3.82</v>
       </c>
-      <c r="U24" s="13">
+      <c r="U24" s="30">
         <v>6.23</v>
       </c>
-      <c r="V24" s="13">
+      <c r="V24" s="30">
         <v>4.37</v>
       </c>
-      <c r="W24" s="13">
+      <c r="W24" s="30">
         <v>3.8</v>
       </c>
-      <c r="X24" s="13">
+      <c r="X24" s="30">
         <v>6.78</v>
       </c>
-      <c r="Y24" s="13">
+      <c r="Y24" s="30">
         <v>4.26</v>
       </c>
-      <c r="Z24" s="13">
+      <c r="Z24" s="30">
         <v>3.6</v>
       </c>
-      <c r="AA24" s="13">
+      <c r="AA24" s="30">
         <v>7.43</v>
       </c>
-      <c r="AB24" s="13">
+      <c r="AB24" s="30">
         <v>4.53</v>
       </c>
-      <c r="AC24" s="13">
+      <c r="AC24" s="30">
         <v>3.87</v>
       </c>
-      <c r="AD24" s="13">
+      <c r="AD24" s="30">
         <v>7.8</v>
       </c>
     </row>
     <row r="25" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="28">
         <v>2.85</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="33">
         <v>2.33</v>
       </c>
-      <c r="F25" s="13">
-        <v>4.25</v>
-      </c>
-      <c r="G25" s="13">
+      <c r="F25" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="28">
         <v>2.8</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H25" s="33">
         <v>2.81</v>
       </c>
-      <c r="I25" s="13">
-        <v>2.77</v>
-      </c>
-      <c r="J25" s="13">
+      <c r="I25" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="28">
         <v>2.5499999999999998</v>
       </c>
-      <c r="K25" s="13">
+      <c r="K25" s="33">
         <v>2.0099999999999998</v>
       </c>
-      <c r="L25" s="13">
-        <v>4.05</v>
-      </c>
-      <c r="M25" s="13">
+      <c r="L25" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="M25" s="28">
         <v>2.56</v>
       </c>
-      <c r="N25" s="13">
+      <c r="N25" s="33">
         <v>2.42</v>
       </c>
-      <c r="O25" s="13">
-        <v>3.01</v>
-      </c>
-      <c r="P25" s="13">
+      <c r="O25" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="P25" s="29">
         <v>2.65</v>
       </c>
-      <c r="Q25" s="13">
+      <c r="Q25" s="34">
         <v>2.4500000000000002</v>
       </c>
-      <c r="R25" s="13">
-        <v>3.37</v>
-      </c>
-      <c r="S25" s="13">
+      <c r="R25" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="S25" s="30">
         <v>2.7</v>
       </c>
-      <c r="T25" s="13">
+      <c r="T25" s="35">
         <v>2.25</v>
       </c>
-      <c r="U25" s="13">
-        <v>4.3600000000000003</v>
-      </c>
-      <c r="V25" s="13">
+      <c r="U25" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="V25" s="30">
         <v>3.52</v>
       </c>
-      <c r="W25" s="13">
+      <c r="W25" s="30">
         <v>3.57</v>
       </c>
-      <c r="X25" s="13">
-        <v>3.38</v>
-      </c>
-      <c r="Y25" s="13">
+      <c r="X25" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y25" s="30">
         <v>3.53</v>
       </c>
-      <c r="Z25" s="13">
+      <c r="Z25" s="30">
         <v>3.22</v>
       </c>
-      <c r="AA25" s="13">
-        <v>4.71</v>
-      </c>
-      <c r="AB25" s="13">
+      <c r="AA25" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB25" s="30">
         <v>4.24</v>
       </c>
-      <c r="AC25" s="13">
+      <c r="AC25" s="30">
         <v>4.4000000000000004</v>
       </c>
-      <c r="AD25" s="13">
+      <c r="AD25" s="37">
         <v>3.63</v>
       </c>
     </row>
     <row r="26" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="28">
         <v>2.41</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="33">
         <v>2.14</v>
       </c>
-      <c r="F26" s="13">
-        <v>3.09</v>
-      </c>
-      <c r="G26" s="13">
+      <c r="F26" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="28">
         <v>2.98</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H26" s="33">
         <v>2.5099999999999998</v>
       </c>
-      <c r="I26" s="13">
+      <c r="I26" s="33">
         <v>4.0999999999999996</v>
       </c>
-      <c r="J26" s="13">
+      <c r="J26" s="28">
         <v>3.07</v>
       </c>
-      <c r="K26" s="13">
+      <c r="K26" s="33">
         <v>2.75</v>
       </c>
-      <c r="L26" s="13">
+      <c r="L26" s="33">
         <v>3.84</v>
       </c>
-      <c r="M26" s="13">
+      <c r="M26" s="28">
         <v>3.56</v>
       </c>
-      <c r="N26" s="13">
+      <c r="N26" s="28">
         <v>3.45</v>
       </c>
-      <c r="O26" s="13">
-        <v>3.9</v>
-      </c>
-      <c r="P26" s="13">
+      <c r="O26" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="P26" s="29">
         <v>3.37</v>
       </c>
-      <c r="Q26" s="13">
+      <c r="Q26" s="34">
         <v>2.6</v>
       </c>
-      <c r="R26" s="13">
+      <c r="R26" s="34">
         <v>5.88</v>
       </c>
-      <c r="S26" s="13">
+      <c r="S26" s="30">
         <v>3.99</v>
       </c>
-      <c r="T26" s="13">
+      <c r="T26" s="30">
         <v>3.65</v>
       </c>
-      <c r="U26" s="13">
+      <c r="U26" s="35">
         <v>5.13</v>
       </c>
-      <c r="V26" s="13">
+      <c r="V26" s="30">
         <v>3.76</v>
       </c>
-      <c r="W26" s="13">
+      <c r="W26" s="30">
         <v>3.57</v>
       </c>
-      <c r="X26" s="13">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="Y26" s="13">
+      <c r="X26" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y26" s="30">
         <v>3.82</v>
       </c>
-      <c r="Z26" s="13">
+      <c r="Z26" s="30">
         <v>3.42</v>
       </c>
-      <c r="AA26" s="13">
+      <c r="AA26" s="32">
         <v>5.15</v>
       </c>
-      <c r="AB26" s="13">
+      <c r="AB26" s="30">
         <v>4.84</v>
       </c>
-      <c r="AC26" s="13">
+      <c r="AC26" s="30">
         <v>4.74</v>
       </c>
-      <c r="AD26" s="13">
+      <c r="AD26" s="30">
         <v>5.2</v>
       </c>
     </row>
     <row r="27" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="13">
-        <v>2.04</v>
-      </c>
-      <c r="E27" s="13">
+      <c r="D27" s="33">
+        <v>2</v>
+      </c>
+      <c r="E27" s="33">
         <v>1.52</v>
       </c>
-      <c r="F27" s="13">
-        <v>3.29</v>
-      </c>
-      <c r="G27" s="13">
+      <c r="F27" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="33">
         <v>1.92</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H27" s="33">
         <v>1.3</v>
       </c>
-      <c r="I27" s="13">
-        <v>3.4</v>
-      </c>
-      <c r="J27" s="13">
+      <c r="I27" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J27" s="28">
         <v>2.77</v>
       </c>
-      <c r="K27" s="13">
+      <c r="K27" s="33">
         <v>2.11</v>
       </c>
-      <c r="L27" s="13">
+      <c r="L27" s="33">
         <v>4.41</v>
       </c>
-      <c r="M27" s="13">
+      <c r="M27" s="28">
         <v>2.5299999999999998</v>
       </c>
-      <c r="N27" s="13">
+      <c r="N27" s="33">
         <v>2</v>
       </c>
-      <c r="O27" s="13">
-        <v>4.16</v>
-      </c>
-      <c r="P27" s="13">
+      <c r="O27" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="P27" s="29">
         <v>3.15</v>
       </c>
-      <c r="Q27" s="13">
+      <c r="Q27" s="29">
         <v>2.71</v>
       </c>
-      <c r="R27" s="13">
+      <c r="R27" s="34">
         <v>4.66</v>
       </c>
-      <c r="S27" s="13">
+      <c r="S27" s="30">
         <v>3.11</v>
       </c>
-      <c r="T27" s="13">
+      <c r="T27" s="30">
         <v>2.77</v>
       </c>
-      <c r="U27" s="13">
-        <v>4.38</v>
-      </c>
-      <c r="V27" s="13">
+      <c r="U27" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="V27" s="30">
         <v>3.34</v>
       </c>
-      <c r="W27" s="13">
+      <c r="W27" s="30">
         <v>3.08</v>
       </c>
-      <c r="X27" s="13">
-        <v>4.37</v>
-      </c>
-      <c r="Y27" s="13">
+      <c r="X27" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y27" s="30">
         <v>3.13</v>
       </c>
-      <c r="Z27" s="13">
+      <c r="Z27" s="30">
         <v>2.99</v>
       </c>
-      <c r="AA27" s="13">
-        <v>3.79</v>
-      </c>
-      <c r="AB27" s="13">
+      <c r="AA27" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB27" s="30">
         <v>3.74</v>
       </c>
-      <c r="AC27" s="13">
+      <c r="AC27" s="30">
         <v>3.28</v>
       </c>
-      <c r="AD27" s="13">
+      <c r="AD27" s="30">
         <v>5.9</v>
       </c>
     </row>
     <row r="28" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="13">
-        <v>1.36</v>
-      </c>
-      <c r="E28" s="13">
-        <v>1.02</v>
-      </c>
-      <c r="F28" s="13">
-        <v>2.86</v>
-      </c>
-      <c r="G28" s="13">
+      <c r="D28" s="33">
+        <v>1.4</v>
+      </c>
+      <c r="E28" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="28">
         <v>1.84</v>
       </c>
-      <c r="H28" s="13">
+      <c r="H28" s="33">
         <v>1.51</v>
       </c>
-      <c r="I28" s="13">
-        <v>3.33</v>
-      </c>
-      <c r="J28" s="13">
+      <c r="I28" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="28">
         <v>2.09</v>
       </c>
-      <c r="K28" s="13">
+      <c r="K28" s="33">
         <v>1.7</v>
       </c>
-      <c r="L28" s="13">
-        <v>4.01</v>
-      </c>
-      <c r="M28" s="13">
+      <c r="L28" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="M28" s="28">
         <v>2.02</v>
       </c>
-      <c r="N28" s="13">
+      <c r="N28" s="28">
         <v>1.91</v>
       </c>
-      <c r="O28" s="13">
-        <v>2.69</v>
-      </c>
-      <c r="P28" s="13">
+      <c r="O28" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="P28" s="29">
         <v>3.03</v>
       </c>
-      <c r="Q28" s="13">
+      <c r="Q28" s="29">
         <v>2.79</v>
       </c>
-      <c r="R28" s="13">
-        <v>4.54</v>
-      </c>
-      <c r="S28" s="13">
+      <c r="R28" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="S28" s="30">
         <v>3.01</v>
       </c>
-      <c r="T28" s="13">
+      <c r="T28" s="30">
         <v>2.74</v>
       </c>
-      <c r="U28" s="13">
-        <v>4.67</v>
-      </c>
-      <c r="V28" s="13">
+      <c r="U28" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="V28" s="30">
         <v>3.18</v>
       </c>
-      <c r="W28" s="13">
+      <c r="W28" s="30">
         <v>2.94</v>
       </c>
-      <c r="X28" s="13">
-        <v>4.55</v>
-      </c>
-      <c r="Y28" s="13">
+      <c r="X28" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y28" s="30">
         <v>3.38</v>
       </c>
-      <c r="Z28" s="13">
+      <c r="Z28" s="30">
         <v>3.03</v>
       </c>
-      <c r="AA28" s="13">
+      <c r="AA28" s="32">
         <v>5.5</v>
       </c>
-      <c r="AB28" s="13">
+      <c r="AB28" s="30">
         <v>3.92</v>
       </c>
-      <c r="AC28" s="13">
+      <c r="AC28" s="30">
         <v>3.65</v>
       </c>
-      <c r="AD28" s="13">
+      <c r="AD28" s="30">
         <v>5.58</v>
       </c>
     </row>
     <row r="29" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="33">
         <v>1.35</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="33">
         <v>1.27</v>
       </c>
-      <c r="F29" s="13">
-        <v>1.84</v>
-      </c>
-      <c r="G29" s="13">
+      <c r="F29" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="33">
         <v>1.58</v>
       </c>
-      <c r="H29" s="13">
+      <c r="H29" s="33">
         <v>1.55</v>
       </c>
-      <c r="I29" s="13">
-        <v>1.78</v>
-      </c>
-      <c r="J29" s="13">
+      <c r="I29" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" s="28">
         <v>1.94</v>
       </c>
-      <c r="K29" s="13">
+      <c r="K29" s="33">
         <v>1.75</v>
       </c>
-      <c r="L29" s="13">
-        <v>2.97</v>
-      </c>
-      <c r="M29" s="13">
+      <c r="L29" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="M29" s="28">
         <v>1.95</v>
       </c>
-      <c r="N29" s="13">
+      <c r="N29" s="33">
         <v>1.67</v>
       </c>
-      <c r="O29" s="13">
-        <v>3.54</v>
-      </c>
-      <c r="P29" s="13">
+      <c r="O29" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="P29" s="29">
         <v>2.09</v>
       </c>
-      <c r="Q29" s="13">
+      <c r="Q29" s="34">
         <v>1.95</v>
       </c>
-      <c r="R29" s="13">
-        <v>2.89</v>
-      </c>
-      <c r="S29" s="13">
+      <c r="R29" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="S29" s="30">
         <v>2.33</v>
       </c>
-      <c r="T29" s="13">
+      <c r="T29" s="35">
         <v>2.14</v>
       </c>
-      <c r="U29" s="13">
-        <v>3.47</v>
-      </c>
-      <c r="V29" s="13">
+      <c r="U29" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="V29" s="30">
         <v>2.6</v>
       </c>
-      <c r="W29" s="13">
+      <c r="W29" s="30">
         <v>2.56</v>
       </c>
-      <c r="X29" s="13">
-        <v>2.86</v>
-      </c>
-      <c r="Y29" s="13">
+      <c r="X29" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y29" s="30">
         <v>2.5099999999999998</v>
       </c>
-      <c r="Z29" s="13">
+      <c r="Z29" s="32">
         <v>2.16</v>
       </c>
-      <c r="AA29" s="13">
-        <v>4.74</v>
-      </c>
-      <c r="AB29" s="13">
+      <c r="AA29" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB29" s="30">
         <v>3.1</v>
       </c>
-      <c r="AC29" s="13">
+      <c r="AC29" s="30">
         <v>2.56</v>
       </c>
-      <c r="AD29" s="13">
+      <c r="AD29" s="37">
         <v>6.58</v>
       </c>
     </row>
     <row r="30" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="28">
         <v>1.91</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="28">
         <v>1.55</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F30" s="28">
         <v>3.13</v>
       </c>
-      <c r="G30" s="13">
+      <c r="G30" s="28">
         <v>2.15</v>
       </c>
-      <c r="H30" s="13">
+      <c r="H30" s="28">
         <v>1.85</v>
       </c>
-      <c r="I30" s="13">
+      <c r="I30" s="28">
         <v>3.19</v>
       </c>
-      <c r="J30" s="13">
+      <c r="J30" s="28">
         <v>2.4300000000000002</v>
       </c>
-      <c r="K30" s="13">
+      <c r="K30" s="28">
         <v>2</v>
       </c>
-      <c r="L30" s="13">
+      <c r="L30" s="28">
         <v>3.91</v>
       </c>
-      <c r="M30" s="13">
+      <c r="M30" s="28">
         <v>2.46</v>
       </c>
-      <c r="N30" s="13">
+      <c r="N30" s="28">
         <v>2.2000000000000002</v>
       </c>
-      <c r="O30" s="13">
+      <c r="O30" s="28">
         <v>3.5</v>
       </c>
-      <c r="P30" s="13">
+      <c r="P30" s="29">
         <v>2.85</v>
       </c>
-      <c r="Q30" s="13">
+      <c r="Q30" s="29">
         <v>2.5</v>
       </c>
-      <c r="R30" s="13">
+      <c r="R30" s="29">
         <v>4.37</v>
       </c>
-      <c r="S30" s="13">
+      <c r="S30" s="30">
         <v>3.01</v>
       </c>
-      <c r="T30" s="13">
+      <c r="T30" s="30">
         <v>2.69</v>
       </c>
-      <c r="U30" s="13">
+      <c r="U30" s="30">
         <v>4.45</v>
       </c>
-      <c r="V30" s="13">
+      <c r="V30" s="30">
         <v>3.25</v>
       </c>
-      <c r="W30" s="13">
+      <c r="W30" s="30">
         <v>3.08</v>
       </c>
-      <c r="X30" s="13">
+      <c r="X30" s="30">
         <v>3.97</v>
       </c>
-      <c r="Y30" s="13">
+      <c r="Y30" s="30">
         <v>3.26</v>
       </c>
-      <c r="Z30" s="13">
+      <c r="Z30" s="30">
         <v>2.94</v>
       </c>
-      <c r="AA30" s="13">
+      <c r="AA30" s="32">
         <v>4.79</v>
       </c>
-      <c r="AB30" s="13">
+      <c r="AB30" s="30">
         <v>3.93</v>
       </c>
-      <c r="AC30" s="13">
+      <c r="AC30" s="30">
         <v>3.65</v>
       </c>
-      <c r="AD30" s="13">
+      <c r="AD30" s="37">
         <v>5.32</v>
       </c>
     </row>
     <row r="31" spans="1:30" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="15"/>
+      <c r="B31" s="12"/>
     </row>
     <row r="32" spans="1:30" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="22"/>
-      <c r="Q32" s="22"/>
-      <c r="R32" s="22"/>
-    </row>
-    <row r="33" spans="2:18" s="16" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="24" t="s">
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+    </row>
+    <row r="33" spans="2:18" s="13" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="25"/>
-      <c r="O33" s="25"/>
-      <c r="P33" s="25"/>
-      <c r="Q33" s="25"/>
-      <c r="R33" s="25"/>
-    </row>
-    <row r="34" spans="2:18" s="16" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="24" t="s">
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="23"/>
+    </row>
+    <row r="34" spans="2:18" s="13" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="23"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="23"/>
-      <c r="P34" s="23"/>
-      <c r="Q34" s="23"/>
-      <c r="R34" s="23"/>
-    </row>
-    <row r="35" spans="2:18" s="16" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="30" t="s">
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+    </row>
+    <row r="35" spans="2:18" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="17"/>
-      <c r="N35" s="17"/>
-      <c r="O35" s="17"/>
-      <c r="P35" s="17"/>
-      <c r="Q35" s="17"/>
-      <c r="R35" s="17"/>
-    </row>
-    <row r="36" spans="2:18" s="16" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
-      <c r="M36" s="17"/>
-      <c r="N36" s="17"/>
-      <c r="O36" s="17"/>
-      <c r="P36" s="17"/>
-      <c r="Q36" s="17"/>
-      <c r="R36" s="17"/>
-    </row>
-    <row r="37" spans="2:18" s="16" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="18" t="s">
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+    </row>
+    <row r="36" spans="2:18" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+    </row>
+    <row r="37" spans="2:18" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="17"/>
-      <c r="O37" s="17"/>
-      <c r="P37" s="17"/>
-      <c r="Q37" s="17"/>
-      <c r="R37" s="17"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
     </row>
     <row r="38" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="19"/>
+      <c r="B38" s="16"/>
     </row>
     <row r="39" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="40" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="17" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="41" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="42" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="39" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="B34:L34"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="M33:R33"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="C6:AD6"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="V7:X7"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="Y7:AA7"/>
+    <mergeCell ref="AB7:AD7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P10"/>
+    <mergeCell ref="AA8:AA9"/>
+    <mergeCell ref="AB8:AB10"/>
+    <mergeCell ref="S8:S10"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="V8:V10"/>
+    <mergeCell ref="W8:W9"/>
     <mergeCell ref="D11:AD11"/>
     <mergeCell ref="AD8:AD9"/>
     <mergeCell ref="E10:F10"/>
@@ -2956,47 +3030,10 @@
     <mergeCell ref="Z8:Z9"/>
     <mergeCell ref="AC8:AC9"/>
     <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S10"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="U8:U9"/>
-    <mergeCell ref="V8:V10"/>
-    <mergeCell ref="W8:W9"/>
-    <mergeCell ref="AB7:AD7"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P10"/>
-    <mergeCell ref="AA8:AA9"/>
-    <mergeCell ref="AB8:AB10"/>
-    <mergeCell ref="B34:L34"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="M33:R33"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="C6:AD6"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="Y7:AA7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B42" r:id="rId1" xr:uid="{FA81AAB6-A221-4AFF-AA2B-88D08CBF9447}"/>
-    <hyperlink ref="B35" r:id="rId2" xr:uid="{188850A0-2492-4A09-9163-26D666064697}"/>
+    <hyperlink ref="B42" r:id="rId1" xr:uid="{FDF3B295-A7FB-4781-AF86-1763E44ECF39}"/>
+    <hyperlink ref="B35" r:id="rId2" xr:uid="{5FAFD498-C3B9-4F1A-A0F4-7857D2E44336}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>